<commit_message>
Anjana's week 10 diary entry
</commit_message>
<xml_diff>
--- a/diaries/diary-anjana-krishnakumar-vellore.xlsx
+++ b/diaries/diary-anjana-krishnakumar-vellore.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Winter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890E29ED-FF62-4746-8AE1-6E0A362D9538}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBE3B96-42F2-4E7B-980B-8F1341DF6A9B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="194">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -197,9 +197,6 @@
     <t>Still feeling nervous about the project</t>
   </si>
   <si>
-    <t xml:space="preserve">Narrowing down one project from a list of possible options was more difficult that expected. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Explored various open source projects available on GitHub, selected OpenRefine and submitted the pull request. </t>
   </si>
   <si>
@@ -234,9 +231,6 @@
     <t>Since we had doubts regarding the project that was initially selected, we decided to try look for more options and to find a new project that is more challenging and interesting than the initial one. We all liked h2 database project and thought it would be interesting to work on databases. Therefore we submitted a new pull request. We also tried to build the project once before submitting the pull request.</t>
   </si>
   <si>
-    <t>Deciding which project to work on was difficult</t>
-  </si>
-  <si>
     <t>12pm - 3pm</t>
   </si>
   <si>
@@ -271,9 +265,6 @@
   </si>
   <si>
     <t>We analysed the selected features using find usage functionality on Intellij to look for possible classes and methods. We also used the templates to keep track of the relevant files we visited. We were also able to figure out where these classes are present in the UML diagram</t>
-  </si>
-  <si>
-    <t>It took a lot of time to figure out where the features are implemented in the code. Templates helped in keeping track of what we were doing</t>
   </si>
   <si>
     <t>Neutral, we think we found relevant classes and methods, but there could be something that we missed out</t>
@@ -325,12 +316,6 @@
     <t>Figure out second feature</t>
   </si>
   <si>
-    <t xml:space="preserve">Some features are very difficult to figure out </t>
-  </si>
-  <si>
-    <t>We were not able to figure out our second feature, even after spending a lot of time and doing a lot of debugging Hence we decided to choose a different feature as our second option which was "How does H2 database handle multiple commands like Insert/Delete etc"</t>
-  </si>
-  <si>
     <t>Slightly nervous if we will be able to complete the homework or not</t>
   </si>
   <si>
@@ -341,9 +326,6 @@
   </si>
   <si>
     <t>Able to understand the flow and we could draw the diagrams</t>
-  </si>
-  <si>
-    <t>It was difficult and had to spend so much time</t>
   </si>
   <si>
     <t>Relaxed as we were able to finally finish the second feature</t>
@@ -515,9 +497,6 @@
     <t>Submit the pull request</t>
   </si>
   <si>
-    <t xml:space="preserve">We realized that certain issues that we thought to be easy were actually not that easy to fix due to either lack of proper test cases or complex dependencies in the codebase. </t>
-  </si>
-  <si>
     <t>The issue was easier to understand because 1)  it was a relatively simple change and had lesser dependencies  2) comments in the pull request were really helpful.</t>
   </si>
   <si>
@@ -541,6 +520,142 @@
   </si>
   <si>
     <t>As Aman and Vaishakhi were not present in the last class, I explained this week's homework. We also discussed couple of possible issues to fix.</t>
+  </si>
+  <si>
+    <t>Learn new concepts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned three more key expert practices and the role of test cases in the process of reverse engineering
+Enjoyed the session conducted by Eric and Michael. Was quite fascinated by their experience and expertise. It was really inspiring. </t>
+  </si>
+  <si>
+    <t>Relieved as we have extra time to complete this week's assignment</t>
+  </si>
+  <si>
+    <t>Understood that testing can help a great deal in understanding the code. For example reading the test cases helps to understand how the system works, running the test cases can help to know which all parts of the code needs to be focused the most and writing the test case would force us to understand the code in greater detail. Understood that test cases play a part in not just validating/verifying the system. It can also play a part in understanding the how the system works</t>
+  </si>
+  <si>
+    <t>11am-12pm</t>
+  </si>
+  <si>
+    <t>Find a second issue (non-trivial) and submit a pull request for the approval</t>
+  </si>
+  <si>
+    <t>We were able to identify a non-trivial issue and submit a pull request</t>
+  </si>
+  <si>
+    <t>ABSENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Could not attend the lecture as I was feeling a bit under the weather and thought it would be better to take rest at home </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asked my friend to explain the topics covered in the class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Felt sad as I missed last lecture. </t>
+  </si>
+  <si>
+    <t>Fix the issue and submit a pull request</t>
+  </si>
+  <si>
+    <t>As we were already familiar with the code base (we had analysed this part for homework 2), we knew which class to look at exactly. So we put our first breakpoint in that class and traced the flow from that point onwards.
+Understood how knowing the essence of a system can help in understanding the system better.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work on second part of this week's assignment - Identifying three interesting test cases and documenting those. </t>
+  </si>
+  <si>
+    <t>We were able to figure out where exactly to make code changes, fixed the issue, tested it and submitted the pull request. We also documented the part in the report</t>
+  </si>
+  <si>
+    <t>Went through the test suite, identified three test cases that we thought were quite interesting and documented the same</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feeling great after completing the second part of the assignment. Only one more part is left. </t>
+  </si>
+  <si>
+    <t>Some features are very difficult to figure out since we are getting lost as we go more and more deeper into the code as we don't have much understanding of the code base yet.</t>
+  </si>
+  <si>
+    <t>9pm - 11pm</t>
+  </si>
+  <si>
+    <t>Work on third part of this week's homework - Create three new test cases
+Finish the report</t>
+  </si>
+  <si>
+    <t>Created three new test cases and finished the report</t>
+  </si>
+  <si>
+    <t>Deciding which project to work on was difficult as we were confused between OpenRefine which is a GUI based application and h2 which is a database (hence not GUI based) . While GUI based applications could be relatively easier to debug and understand, non-GUI based projects would be difficult to understand and hence more challenging. We were little anxious if we would be able to understand a challenging project like h2 in few weeks' time</t>
+  </si>
+  <si>
+    <t>UML class diagrams were not that helpful in understanding this feature as it was difficult to comprehend the UML class diagram since many classes were involved in this feature and we couldn't understand the flow/relations properly from the huge UML. So as we were reading the code and going from one function to the other function, we drew diagrams/graph that represented the flow. This helped in understanding the flow better and we were not lost this time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narrowing down one project from a list of possible options was more difficult that expected as there was lot of good open source projects available, hence we could reach into an agreement only after a long discussion since the team members had different view points. </t>
+  </si>
+  <si>
+    <t>It took a lot of time to figure out where the features are implemented in the code. Templates helped in keeping track of what we were doing as these features were not that big.</t>
+  </si>
+  <si>
+    <t>We were not able to figure out our second feature, even after spending a lot of time and doing a lot of debugging. Hence we decided to choose a different feature (considering the time we have to complete the homework) as our second option which was "How does H2 database handle multiple commands like Insert/Delete etc"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We realized that certain issues that we thought to be easy were actually not that easy to fix due to either lack of proper test cases/examples in the pull request or complex dependencies in the codebase which we were not able to figure out. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happy that our pull request got accepted the same day. 
+</t>
+  </si>
+  <si>
+    <t>We picked the particular issue because 1) the issue has been described properly with a clear test case 2) non-trivial because it involves making changes to the way in which INSERT queries are handled by the h2 databse as this is one of the essential feature of the system
+Fixing this issue could be challenging as this relates to the core functionality of the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We understood that test cases need not essentially be written using unit test frameworks like JUnit. Realised that we could write test cases as regular Java applications
+Although we knew about benchmarking, it is only after going through these tests that we realized the importance of runtime and space complexity analysis (checking for number of statements executed per second and checking for garbage collection limits). We were able to understand how h2 handled this. </t>
+  </si>
+  <si>
+    <t>We were surprised to see that there were many edge cases like referential integrity constraint violation error were not specifically checked by any of the test cases in the existing test suite</t>
+  </si>
+  <si>
+    <t>Go through last lecture's slides</t>
+  </si>
+  <si>
+    <t>Feeling proud after completing the last homework</t>
+  </si>
+  <si>
+    <t>Happy to have gone through the lecture that I missed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glad that we have fixed the issue and submitted the pull request earlier than we expected. Hoping that our pull request gets accepted. </t>
+  </si>
+  <si>
+    <t>2/7/2020 - 2/13/2020</t>
+  </si>
+  <si>
+    <t>Different timings</t>
+  </si>
+  <si>
+    <t>Prepare for the mid term exam</t>
+  </si>
+  <si>
+    <t>Was reviewing the slides and going through my lecture notes to prepare for the mid term exam</t>
+  </si>
+  <si>
+    <t>Hope that I have covered all the topics and prepared well for the exam</t>
+  </si>
+  <si>
+    <t>Lecture notes were really helpful while reviewing the slides as it helped to remember certain examples mentioned in the class</t>
+  </si>
+  <si>
+    <t>Reviewed last lecture's slides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understanding the history of the code base is important to avoid making mistakes while making any changes. We need to respect and understand what is there in the legacy code
+I look forward to apply all the topics (like Key expert practices, principles of reverse engineering, various strategies, tools etc.) I learned in this class. </t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G132"/>
+  <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1356,7 +1471,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>43848</v>
       </c>
@@ -1367,13 +1482,13 @@
         <v>18</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>49</v>
+        <v>174</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>48</v>
@@ -1393,22 +1508,22 @@
         <v>43853</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1420,27 +1535,27 @@
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="202.8" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>43856</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D26" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1457,22 +1572,22 @@
         <v>43856</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1489,22 +1604,22 @@
         <v>43858</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>73</v>
+        <v>175</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1521,22 +1636,22 @@
         <v>43860</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D32" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="G32" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
@@ -1550,16 +1665,16 @@
         <v>15</v>
       </c>
       <c r="D33" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1576,22 +1691,22 @@
         <v>43864</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="F35" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="G35" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1603,27 +1718,27 @@
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="156" x14ac:dyDescent="0.3">
       <c r="A37" s="10">
         <v>43865</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>90</v>
+        <v>176</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>89</v>
+        <v>168</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1635,27 +1750,27 @@
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="234" x14ac:dyDescent="0.3">
       <c r="A39" s="10">
         <v>43866</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>95</v>
+        <v>173</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1672,22 +1787,22 @@
         <v>43867</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1704,22 +1819,22 @@
         <v>43867</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1731,27 +1846,27 @@
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="10">
-        <v>43874</v>
+    <row r="45" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>186</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>52</v>
+        <v>187</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>106</v>
+        <v>188</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>107</v>
+        <v>189</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>108</v>
+        <v>191</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1763,27 +1878,27 @@
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A47" s="10">
-        <v>43877</v>
+        <v>43874</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1795,27 +1910,27 @@
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A49" s="10">
-        <v>43880</v>
+        <v>43877</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>115</v>
+        <v>18</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1827,27 +1942,27 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="249.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A51" s="10">
-        <v>43881</v>
+        <v>43880</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1859,27 +1974,27 @@
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="249.6" x14ac:dyDescent="0.3">
       <c r="A53" s="10">
-        <v>43884</v>
+        <v>43881</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>131</v>
+        <v>14</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1893,25 +2008,25 @@
     </row>
     <row r="55" spans="1:7" ht="156" x14ac:dyDescent="0.3">
       <c r="A55" s="10">
-        <v>43885</v>
+        <v>43884</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1923,27 +2038,27 @@
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="156" x14ac:dyDescent="0.3">
       <c r="A57" s="10">
-        <v>43888</v>
+        <v>43885</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>52</v>
+        <v>128</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1955,27 +2070,27 @@
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A59" s="10">
-        <v>43890</v>
+        <v>43888</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1987,27 +2102,27 @@
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A61" s="10">
-        <v>43891</v>
+        <v>43890</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2019,27 +2134,27 @@
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A63" s="10">
-        <v>43892</v>
+        <v>43891</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2053,25 +2168,25 @@
     </row>
     <row r="65" spans="1:7" ht="78" x14ac:dyDescent="0.3">
       <c r="A65" s="10">
-        <v>43894</v>
+        <v>43892</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -2083,14 +2198,28 @@
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="10"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="8"/>
+    <row r="67" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A67" s="10">
+        <v>43894</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="7"/>
@@ -2101,14 +2230,28 @@
       <c r="F68" s="7"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7"/>
-      <c r="F69" s="7"/>
-      <c r="G69" s="8"/>
+    <row r="69" spans="1:7" ht="249.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="10">
+        <v>43895</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="7"/>
@@ -2119,14 +2262,28 @@
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="7"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7"/>
-      <c r="G71" s="8"/>
+    <row r="71" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="10">
+        <v>43898</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="7"/>
@@ -2137,14 +2294,26 @@
       <c r="F72" s="7"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
+    <row r="73" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A73" s="10">
+        <v>43902</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>160</v>
+      </c>
       <c r="F73" s="7"/>
-      <c r="G73" s="8"/>
+      <c r="G73" s="8" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="7"/>
@@ -2155,14 +2324,28 @@
       <c r="F74" s="7"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="7"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
-      <c r="G75" s="8"/>
+    <row r="75" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+      <c r="A75" s="10">
+        <v>43903</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="7"/>
@@ -2173,14 +2356,28 @@
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="7"/>
-      <c r="F77" s="7"/>
-      <c r="G77" s="8"/>
+    <row r="77" spans="1:7" ht="249.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="10">
+        <v>43904</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="G77" s="8" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="7"/>
@@ -2191,14 +2388,28 @@
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="7"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
-      <c r="G79" s="8"/>
+    <row r="79" spans="1:7" ht="171.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="10">
+        <v>43905</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G79" s="8" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="7"/>
@@ -2209,14 +2420,28 @@
       <c r="F80" s="7"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="7"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
-      <c r="D81" s="7"/>
-      <c r="E81" s="7"/>
-      <c r="F81" s="7"/>
-      <c r="G81" s="8"/>
+    <row r="81" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="10">
+        <v>43905</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="G81" s="8" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="7"/>
@@ -2228,7 +2453,7 @@
       <c r="G82" s="8"/>
     </row>
     <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="7"/>
+      <c r="A83" s="10"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
@@ -2676,6 +2901,42 @@
       <c r="E132" s="7"/>
       <c r="F132" s="7"/>
       <c r="G132" s="8"/>
+    </row>
+    <row r="133" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A133" s="7"/>
+      <c r="B133" s="7"/>
+      <c r="C133" s="7"/>
+      <c r="D133" s="7"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="7"/>
+      <c r="G133" s="8"/>
+    </row>
+    <row r="134" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A134" s="7"/>
+      <c r="B134" s="7"/>
+      <c r="C134" s="7"/>
+      <c r="D134" s="7"/>
+      <c r="E134" s="7"/>
+      <c r="F134" s="7"/>
+      <c r="G134" s="8"/>
+    </row>
+    <row r="135" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A135" s="7"/>
+      <c r="B135" s="7"/>
+      <c r="C135" s="7"/>
+      <c r="D135" s="7"/>
+      <c r="E135" s="7"/>
+      <c r="F135" s="7"/>
+      <c r="G135" s="8"/>
+    </row>
+    <row r="136" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A136" s="7"/>
+      <c r="B136" s="7"/>
+      <c r="C136" s="7"/>
+      <c r="D136" s="7"/>
+      <c r="E136" s="7"/>
+      <c r="F136" s="7"/>
+      <c r="G136" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>